<commit_message>
21 Aug 2023 gblobal chat is working
</commit_message>
<xml_diff>
--- a/dummy/C0_1L976.xlsx
+++ b/dummy/C0_1L976.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\01934L744\Box\Baijnath Data\Project 2023\Nidhi\contract - v4.1\dummy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638FF5CE-A358-4D27-A033-D02B57F99CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5E091F-F310-4DF5-BE03-2D7B25181BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4810" yWindow="2720" windowWidth="14390" windowHeight="7360" xr2:uid="{5E2AB541-C0AE-411E-B46D-9E7337E26435}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5E2AB541-C0AE-411E-B46D-9E7337E26435}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2 (2)" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Hours</t>
   </si>
@@ -62,13 +62,19 @@
     <t>Unit_Of_Measure</t>
   </si>
   <si>
-    <t>Contract_Payterms</t>
-  </si>
-  <si>
     <t>Line_Item_Desc</t>
   </si>
   <si>
     <t>Supplier</t>
+  </si>
+  <si>
+    <t>Payment_Terms_Contract</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
 </sst>
 </file>
@@ -104,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BB26B4-106B-4AAB-80FE-35B262C3ABE2}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -430,71 +437,98 @@
   <cols>
     <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1">
+        <v>41849</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44196</v>
+      </c>
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>150</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>92.4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1">
+        <v>41849</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44196</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>150</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>115.3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>